<commit_message>
Updated sprint burndown to reflect my work across the duration
</commit_message>
<xml_diff>
--- a/documentation/Sprint Backlog  Burndown.xlsx
+++ b/documentation/Sprint Backlog  Burndown.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24326"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/0854baf48ed3e786/Documents/College Docs/Software Engineering/Round 2/Projects/Project 2/GroupPirateShipInventory/documentation/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kdunca10\Downloads\Program Construction\PirateShipProject3\documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="5" documentId="13_ncr:1_{025DB07E-3CC9-4A6A-8309-1B249045E885}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E71FD38E-7AF3-48C0-93E9-7333F965DAFC}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA1E69F0-46A7-4CD7-985E-864C15A6BE2E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="18756" yWindow="17172" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="14010" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -27,8 +27,6 @@
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -36,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="20">
   <si>
     <t>Related User Story</t>
   </si>
@@ -45,18 +43,6 @@
   </si>
   <si>
     <t>Initial Estimate</t>
-  </si>
-  <si>
-    <t>Week 1</t>
-  </si>
-  <si>
-    <t>Week 2</t>
-  </si>
-  <si>
-    <t>Week 3</t>
-  </si>
-  <si>
-    <t>Week 4</t>
   </si>
   <si>
     <t>Amount Remaining After…</t>
@@ -295,10 +281,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -333,6 +318,16 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="16" fontId="1" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -452,13 +447,13 @@
                   <c:v>21</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0</c:v>
+                  <c:v>7</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0</c:v>
+                  <c:v>7</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0</c:v>
+                  <c:v>7</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>0</c:v>
@@ -601,7 +596,6 @@
     </c:plotArea>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
-    <c:showDLblsOverMax val="0"/>
     <c:extLst>
       <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
         <c16r3:dataDisplayOptions16>
@@ -609,6 +603,7 @@
         </c16r3:dataDisplayOptions16>
       </c:ext>
     </c:extLst>
+    <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:spPr>
     <a:solidFill>
@@ -1505,8 +1500,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H27"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="D4" sqref="D4:H4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1519,359 +1514,375 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A1" s="18" t="s">
+      <c r="A1" s="17" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="18" t="s">
+      <c r="B1" s="17" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="18" t="s">
+      <c r="C1" s="17" t="s">
+        <v>5</v>
+      </c>
+      <c r="D1" s="17" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="16" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" s="16"/>
+      <c r="G1" s="16"/>
+      <c r="H1" s="16"/>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2" s="17"/>
+      <c r="B2" s="17"/>
+      <c r="C2" s="17"/>
+      <c r="D2" s="17"/>
+      <c r="E2" s="18">
+        <v>45996</v>
+      </c>
+      <c r="F2" s="18">
+        <v>45997</v>
+      </c>
+      <c r="G2" s="18">
+        <v>45998</v>
+      </c>
+      <c r="H2" s="18">
+        <v>45999</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+      <c r="A3" s="12" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D3" s="3">
+        <v>6</v>
+      </c>
+      <c r="E3" s="4"/>
+      <c r="F3" s="4"/>
+      <c r="G3" s="4"/>
+      <c r="H3" s="4"/>
+    </row>
+    <row r="4" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+      <c r="A4" s="13"/>
+      <c r="B4" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="D1" s="18" t="s">
+      <c r="C4" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D4" s="21">
+        <v>3</v>
+      </c>
+      <c r="E4" s="19">
+        <v>3</v>
+      </c>
+      <c r="F4" s="19">
+        <v>3</v>
+      </c>
+      <c r="G4" s="19">
+        <v>3</v>
+      </c>
+      <c r="H4" s="19">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A5" s="13"/>
+      <c r="B5" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="D5" s="3">
+        <v>1</v>
+      </c>
+      <c r="E5" s="4"/>
+      <c r="F5" s="4"/>
+      <c r="G5" s="4"/>
+      <c r="H5" s="4"/>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A6" s="13"/>
+      <c r="B6" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="D6" s="3">
         <v>2</v>
       </c>
-      <c r="E1" s="17" t="s">
+      <c r="E6" s="4"/>
+      <c r="F6" s="4"/>
+      <c r="G6" s="4"/>
+      <c r="H6" s="4"/>
+    </row>
+    <row r="7" spans="1:8" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="14"/>
+      <c r="B7" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="C7" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="F1" s="17"/>
-      <c r="G1" s="17"/>
-      <c r="H1" s="17"/>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A2" s="18"/>
-      <c r="B2" s="18"/>
-      <c r="C2" s="18"/>
-      <c r="D2" s="18"/>
-      <c r="E2" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="F2" s="2" t="s">
+      <c r="D7" s="9">
+        <v>1</v>
+      </c>
+      <c r="E7" s="4"/>
+      <c r="F7" s="4"/>
+      <c r="G7" s="4"/>
+      <c r="H7" s="4"/>
+    </row>
+    <row r="8" spans="1:8" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="B8" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="C8" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="D8" s="20">
         <v>4</v>
       </c>
-      <c r="G2" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="H2" s="2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" ht="45" x14ac:dyDescent="0.25">
-      <c r="A3" s="13" t="s">
+      <c r="E8" s="19">
+        <v>4</v>
+      </c>
+      <c r="F8" s="19">
+        <v>4</v>
+      </c>
+      <c r="G8" s="19">
+        <v>4</v>
+      </c>
+      <c r="H8" s="19">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" ht="28.9" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="15" t="s">
+        <v>17</v>
+      </c>
+      <c r="B9" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="C9" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="B3" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="C3" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="D3" s="4">
-        <v>6</v>
-      </c>
-      <c r="E3" s="5"/>
-      <c r="F3" s="5"/>
-      <c r="G3" s="5"/>
-      <c r="H3" s="5"/>
-    </row>
-    <row r="4" spans="1:8" ht="45" x14ac:dyDescent="0.25">
-      <c r="A4" s="14"/>
-      <c r="B4" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="C4" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="D4" s="4">
-        <v>3</v>
-      </c>
-      <c r="E4" s="5"/>
-      <c r="F4" s="5"/>
-      <c r="G4" s="5"/>
-      <c r="H4" s="5"/>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A5" s="14"/>
-      <c r="B5" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="C5" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="D5" s="4">
-        <v>1</v>
-      </c>
-      <c r="E5" s="5"/>
-      <c r="F5" s="5"/>
-      <c r="G5" s="5"/>
-      <c r="H5" s="5"/>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A6" s="14"/>
-      <c r="B6" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="C6" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="D6" s="4">
+      <c r="D9" s="7">
         <v>2</v>
       </c>
-      <c r="E6" s="5"/>
-      <c r="F6" s="5"/>
-      <c r="G6" s="5"/>
-      <c r="H6" s="5"/>
-    </row>
-    <row r="7" spans="1:8" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="15"/>
-      <c r="B7" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="C7" s="10" t="s">
-        <v>11</v>
-      </c>
-      <c r="D7" s="10">
-        <v>1</v>
-      </c>
-      <c r="E7" s="5"/>
-      <c r="F7" s="5"/>
-      <c r="G7" s="5"/>
-      <c r="H7" s="5"/>
-    </row>
-    <row r="8" spans="1:8" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="11" t="s">
+      <c r="E9" s="4"/>
+      <c r="F9" s="4"/>
+      <c r="G9" s="4"/>
+      <c r="H9" s="4"/>
+    </row>
+    <row r="10" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="14"/>
+      <c r="B10" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="B8" s="12" t="s">
-        <v>20</v>
-      </c>
-      <c r="C8" s="12" t="s">
-        <v>14</v>
-      </c>
-      <c r="D8" s="12">
+      <c r="C10" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="D10" s="9">
+        <v>2</v>
+      </c>
+      <c r="E10" s="4"/>
+      <c r="F10" s="4"/>
+      <c r="G10" s="4"/>
+      <c r="H10" s="4"/>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A11" s="7"/>
+      <c r="B11" s="7"/>
+      <c r="C11" s="7"/>
+      <c r="D11" s="7"/>
+      <c r="E11" s="4"/>
+      <c r="F11" s="4"/>
+      <c r="G11" s="4"/>
+      <c r="H11" s="4"/>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A12" s="3"/>
+      <c r="B12" s="3"/>
+      <c r="C12" s="3"/>
+      <c r="D12" s="3"/>
+      <c r="E12" s="4"/>
+      <c r="F12" s="4"/>
+      <c r="G12" s="4"/>
+      <c r="H12" s="4"/>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A13" s="3"/>
+      <c r="B13" s="3"/>
+      <c r="C13" s="3"/>
+      <c r="D13" s="3"/>
+      <c r="E13" s="4"/>
+      <c r="F13" s="4"/>
+      <c r="G13" s="4"/>
+      <c r="H13" s="4"/>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A14" s="3"/>
+      <c r="B14" s="3"/>
+      <c r="C14" s="3"/>
+      <c r="D14" s="3"/>
+      <c r="E14" s="4"/>
+      <c r="F14" s="4"/>
+      <c r="G14" s="4"/>
+      <c r="H14" s="4"/>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A15" s="3"/>
+      <c r="B15" s="3"/>
+      <c r="C15" s="3"/>
+      <c r="D15" s="3"/>
+      <c r="E15" s="4"/>
+      <c r="F15" s="4"/>
+      <c r="G15" s="4"/>
+      <c r="H15" s="4"/>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A16" s="3"/>
+      <c r="B16" s="3"/>
+      <c r="C16" s="3"/>
+      <c r="D16" s="3"/>
+      <c r="E16" s="4"/>
+      <c r="F16" s="4"/>
+      <c r="G16" s="4"/>
+      <c r="H16" s="4"/>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A17" s="3"/>
+      <c r="B17" s="3"/>
+      <c r="C17" s="3"/>
+      <c r="D17" s="3"/>
+      <c r="E17" s="4"/>
+      <c r="F17" s="4"/>
+      <c r="G17" s="4"/>
+      <c r="H17" s="4"/>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A18" s="3"/>
+      <c r="B18" s="3"/>
+      <c r="C18" s="3"/>
+      <c r="D18" s="3"/>
+      <c r="E18" s="4"/>
+      <c r="F18" s="4"/>
+      <c r="G18" s="4"/>
+      <c r="H18" s="4"/>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A19" s="3"/>
+      <c r="B19" s="3"/>
+      <c r="C19" s="3"/>
+      <c r="D19" s="3"/>
+      <c r="E19" s="4"/>
+      <c r="F19" s="4"/>
+      <c r="G19" s="4"/>
+      <c r="H19" s="4"/>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A20" s="3"/>
+      <c r="B20" s="3"/>
+      <c r="C20" s="3"/>
+      <c r="D20" s="3"/>
+      <c r="E20" s="4"/>
+      <c r="F20" s="4"/>
+      <c r="G20" s="4"/>
+      <c r="H20" s="4"/>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A21" s="3"/>
+      <c r="B21" s="3"/>
+      <c r="C21" s="3"/>
+      <c r="D21" s="3"/>
+      <c r="E21" s="4"/>
+      <c r="F21" s="4"/>
+      <c r="G21" s="4"/>
+      <c r="H21" s="4"/>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A22" s="3"/>
+      <c r="B22" s="3"/>
+      <c r="C22" s="3"/>
+      <c r="D22" s="3"/>
+      <c r="E22" s="4"/>
+      <c r="F22" s="4"/>
+      <c r="G22" s="4"/>
+      <c r="H22" s="4"/>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A23" s="3"/>
+      <c r="B23" s="3"/>
+      <c r="C23" s="3"/>
+      <c r="D23" s="3"/>
+      <c r="E23" s="4"/>
+      <c r="F23" s="4"/>
+      <c r="G23" s="4"/>
+      <c r="H23" s="4"/>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A24" s="3"/>
+      <c r="B24" s="3"/>
+      <c r="C24" s="3"/>
+      <c r="D24" s="3"/>
+      <c r="E24" s="4"/>
+      <c r="F24" s="4"/>
+      <c r="G24" s="4"/>
+      <c r="H24" s="4"/>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A25" s="3"/>
+      <c r="B25" s="3"/>
+      <c r="C25" s="3"/>
+      <c r="D25" s="3"/>
+      <c r="E25" s="4"/>
+      <c r="F25" s="4"/>
+      <c r="G25" s="4"/>
+      <c r="H25" s="4"/>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A26" s="3"/>
+      <c r="B26" s="3"/>
+      <c r="C26" s="3"/>
+      <c r="D26" s="3"/>
+      <c r="E26" s="4"/>
+      <c r="F26" s="4"/>
+      <c r="G26" s="4"/>
+      <c r="H26" s="4"/>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B27" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="E8" s="5"/>
-      <c r="F8" s="5"/>
-      <c r="G8" s="5"/>
-      <c r="H8" s="5"/>
-    </row>
-    <row r="9" spans="1:8" ht="28.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="16" t="s">
-        <v>21</v>
-      </c>
-      <c r="B9" s="8" t="s">
-        <v>22</v>
-      </c>
-      <c r="C9" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="D9" s="8">
-        <v>2</v>
-      </c>
-      <c r="E9" s="5"/>
-      <c r="F9" s="5"/>
-      <c r="G9" s="5"/>
-      <c r="H9" s="5"/>
-    </row>
-    <row r="10" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="15"/>
-      <c r="B10" s="10" t="s">
-        <v>23</v>
-      </c>
-      <c r="C10" s="10" t="s">
-        <v>16</v>
-      </c>
-      <c r="D10" s="10">
-        <v>2</v>
-      </c>
-      <c r="E10" s="5"/>
-      <c r="F10" s="5"/>
-      <c r="G10" s="5"/>
-      <c r="H10" s="5"/>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A11" s="8"/>
-      <c r="B11" s="8"/>
-      <c r="C11" s="8"/>
-      <c r="D11" s="8"/>
-      <c r="E11" s="5"/>
-      <c r="F11" s="5"/>
-      <c r="G11" s="5"/>
-      <c r="H11" s="5"/>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A12" s="4"/>
-      <c r="B12" s="4"/>
-      <c r="C12" s="4"/>
-      <c r="D12" s="4"/>
-      <c r="E12" s="5"/>
-      <c r="F12" s="5"/>
-      <c r="G12" s="5"/>
-      <c r="H12" s="5"/>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A13" s="4"/>
-      <c r="B13" s="4"/>
-      <c r="C13" s="4"/>
-      <c r="D13" s="4"/>
-      <c r="E13" s="5"/>
-      <c r="F13" s="5"/>
-      <c r="G13" s="5"/>
-      <c r="H13" s="5"/>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A14" s="4"/>
-      <c r="B14" s="4"/>
-      <c r="C14" s="4"/>
-      <c r="D14" s="4"/>
-      <c r="E14" s="5"/>
-      <c r="F14" s="5"/>
-      <c r="G14" s="5"/>
-      <c r="H14" s="5"/>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A15" s="4"/>
-      <c r="B15" s="4"/>
-      <c r="C15" s="4"/>
-      <c r="D15" s="4"/>
-      <c r="E15" s="5"/>
-      <c r="F15" s="5"/>
-      <c r="G15" s="5"/>
-      <c r="H15" s="5"/>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A16" s="4"/>
-      <c r="B16" s="4"/>
-      <c r="C16" s="4"/>
-      <c r="D16" s="4"/>
-      <c r="E16" s="5"/>
-      <c r="F16" s="5"/>
-      <c r="G16" s="5"/>
-      <c r="H16" s="5"/>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A17" s="4"/>
-      <c r="B17" s="4"/>
-      <c r="C17" s="4"/>
-      <c r="D17" s="4"/>
-      <c r="E17" s="5"/>
-      <c r="F17" s="5"/>
-      <c r="G17" s="5"/>
-      <c r="H17" s="5"/>
-    </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A18" s="4"/>
-      <c r="B18" s="4"/>
-      <c r="C18" s="4"/>
-      <c r="D18" s="4"/>
-      <c r="E18" s="5"/>
-      <c r="F18" s="5"/>
-      <c r="G18" s="5"/>
-      <c r="H18" s="5"/>
-    </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A19" s="4"/>
-      <c r="B19" s="4"/>
-      <c r="C19" s="4"/>
-      <c r="D19" s="4"/>
-      <c r="E19" s="5"/>
-      <c r="F19" s="5"/>
-      <c r="G19" s="5"/>
-      <c r="H19" s="5"/>
-    </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A20" s="4"/>
-      <c r="B20" s="4"/>
-      <c r="C20" s="4"/>
-      <c r="D20" s="4"/>
-      <c r="E20" s="5"/>
-      <c r="F20" s="5"/>
-      <c r="G20" s="5"/>
-      <c r="H20" s="5"/>
-    </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A21" s="4"/>
-      <c r="B21" s="4"/>
-      <c r="C21" s="4"/>
-      <c r="D21" s="4"/>
-      <c r="E21" s="5"/>
-      <c r="F21" s="5"/>
-      <c r="G21" s="5"/>
-      <c r="H21" s="5"/>
-    </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A22" s="4"/>
-      <c r="B22" s="4"/>
-      <c r="C22" s="4"/>
-      <c r="D22" s="4"/>
-      <c r="E22" s="5"/>
-      <c r="F22" s="5"/>
-      <c r="G22" s="5"/>
-      <c r="H22" s="5"/>
-    </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A23" s="4"/>
-      <c r="B23" s="4"/>
-      <c r="C23" s="4"/>
-      <c r="D23" s="4"/>
-      <c r="E23" s="5"/>
-      <c r="F23" s="5"/>
-      <c r="G23" s="5"/>
-      <c r="H23" s="5"/>
-    </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A24" s="4"/>
-      <c r="B24" s="4"/>
-      <c r="C24" s="4"/>
-      <c r="D24" s="4"/>
-      <c r="E24" s="5"/>
-      <c r="F24" s="5"/>
-      <c r="G24" s="5"/>
-      <c r="H24" s="5"/>
-    </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A25" s="4"/>
-      <c r="B25" s="4"/>
-      <c r="C25" s="4"/>
-      <c r="D25" s="4"/>
-      <c r="E25" s="5"/>
-      <c r="F25" s="5"/>
-      <c r="G25" s="5"/>
-      <c r="H25" s="5"/>
-    </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A26" s="4"/>
-      <c r="B26" s="4"/>
-      <c r="C26" s="4"/>
-      <c r="D26" s="4"/>
-      <c r="E26" s="5"/>
-      <c r="F26" s="5"/>
-      <c r="G26" s="5"/>
-      <c r="H26" s="5"/>
-    </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B27" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="C27" s="6"/>
-      <c r="D27" s="7">
+      <c r="C27" s="5"/>
+      <c r="D27" s="6">
         <f>SUM(D3:D26)</f>
         <v>21</v>
       </c>
-      <c r="E27" s="7">
+      <c r="E27" s="6">
         <f t="shared" ref="E27:H27" si="0">SUM(E3:E26)</f>
-        <v>0</v>
-      </c>
-      <c r="F27" s="7">
+        <v>7</v>
+      </c>
+      <c r="F27" s="6">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="G27" s="7">
+        <v>7</v>
+      </c>
+      <c r="G27" s="6">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="H27" s="7">
+        <v>7</v>
+      </c>
+      <c r="H27" s="6">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>

</xml_diff>